<commit_message>
Added POST_GET_DELETE custom filter 5 test cases
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/POST_GET_DELETE_Filter.xlsx
+++ b/BloodstreamAPI/testData/POST_GET_DELETE_Filter.xlsx
@@ -3,12 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2051DCDF-7F8B-4BC4-A94D-49E96759A75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B29B42-1C7D-4AF9-91B5-A5E253FBCCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FilterActions" sheetId="24" r:id="rId1"/>
+    <sheet name="ConcApproveGrid" sheetId="24" r:id="rId1"/>
+    <sheet name="DonationGrid" sheetId="25" r:id="rId2"/>
+    <sheet name="TestGrid" sheetId="26" r:id="rId3"/>
+    <sheet name="WorklistInfGrid" sheetId="27" r:id="rId4"/>
+    <sheet name="WorklistConcGrid" sheetId="28" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="16">
   <si>
     <t>EndPoint</t>
   </si>
@@ -37,16 +41,37 @@
     <t>ConclusionsToApprove</t>
   </si>
   <si>
-    <t>POSTFilterAssert200</t>
-  </si>
-  <si>
     <t>GETFilterAssert200</t>
   </si>
   <si>
     <t>DeleteFilterAssert200</t>
   </si>
   <si>
+    <t>Assert200</t>
+  </si>
+  <si>
+    <t>DonationInformation</t>
+  </si>
+  <si>
+    <t>TestInformation</t>
+  </si>
+  <si>
+    <t>WorklistInformation</t>
+  </si>
+  <si>
+    <t>WorklistConclusions</t>
+  </si>
+  <si>
+    <t>V0MxMjM0Kio=</t>
+  </si>
+  <si>
     <t>Q3VzdG9tMUAjJF4k</t>
+  </si>
+  <si>
+    <t>V08xMjM0Kio=</t>
+  </si>
+  <si>
+    <t>dGVzdGluZzEyMzAq</t>
   </si>
 </sst>
 </file>
@@ -104,7 +129,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -126,6 +151,10 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -419,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BCC6FA-DE2E-4F4B-A5A9-89B1733852E0}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +461,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4"/>
     </row>
@@ -458,11 +487,11 @@
       <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -483,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -492,11 +521,11 @@
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -517,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -529,6 +558,454 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B95ED9B-D37B-4023-AD18-22E81E822C30}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CACF74-8710-4011-9C5A-88142DC82A7C}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A115630-1F90-4908-8C34-71B646CFCB33}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17F7E5E-2A57-4BF2-9800-07FE2F5B30B1}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="46.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>